<commit_message>
updated financialfianncial and enrollment
</commit_message>
<xml_diff>
--- a/output_cash_flow/all_schools.xlsx
+++ b/output_cash_flow/all_schools.xlsx
@@ -9,15 +9,23 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ARIZONA_STATE_UNIVERSITY" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BRADLEY_UNIVERSITY" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CORNELL_UNIVERSITY" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GANNON_UNIVERSITY" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LEWIS_UNIVERSITY" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MOLLOY_COLLEGE" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW_YORK_UNIVERSITY" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRESIDENT___FELLOWS_OF_HARVARD_" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STEVENSON_UNIVERSITY_INC" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STEVENS_INSTITUTE_OF_TECHNOLOGY" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ST_LOUIS_UNIVERSITY_US" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CALIFORNIA_STATE_UNIVERSITY" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CORNELL_UNIVERSITY" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CULINARY_INSTITUTE_OF_AMERICA_T" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GANNON_UNIVERSITY" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LEWIS_UNIVERSITY" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MICHIGAN_STATE_UNIVERSITY" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MOLLOY_COLLEGE" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MOUNT_ST_MARY_S_UNIVERSITY_INC" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW_YORK_UNIVERSITY" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OHIO_STATE_UNIVERSITY_THE" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PRESIDENT___FELLOWS_OF_HARVARD_" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STEVENSON_UNIVERSITY_INC" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STEVENS_INSTITUTE_OF_TECHNOLOGY" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ST_LOUIS_UNIVERSITY_US" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TEXAS_A_M_UNIVERSITY" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNIVERSITY_OF_COLORADO" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UNIVERSITY_OF_MINNESOTA" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,7 +470,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>194089</v>
+        <v>194089000</v>
       </c>
     </row>
     <row r="3">
@@ -472,7 +480,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>220984</v>
+        <v>220984000</v>
       </c>
     </row>
     <row r="4">
@@ -498,7 +506,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-655833000</v>
+        <v>-655833</v>
       </c>
     </row>
     <row r="7">
@@ -508,7 +516,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-466593309</v>
+        <v>466829</v>
       </c>
     </row>
     <row r="8">
@@ -526,7 +534,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>54813000</v>
+        <v>54813</v>
       </c>
     </row>
     <row r="10">
@@ -536,7 +544,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>342354000</v>
+        <v>342354</v>
       </c>
     </row>
     <row r="11">
@@ -546,7 +554,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-120612396</v>
+        <v>120964</v>
       </c>
     </row>
     <row r="12">
@@ -555,9 +563,7 @@
           <t>change_in_long_term_debt</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>232635</v>
-      </c>
+      <c r="B12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -573,7 +579,9 @@
           <t>net_cash_from_financing_activities</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>679424</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -582,7 +590,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>78400000</v>
+        <v>78400</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +630,9 @@
           <t>total_change_in_net_assets</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>6951753</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -630,7 +640,9 @@
           <t>total_non_cash_exp</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="n">
+        <v>7514013</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -654,7 +666,9 @@
           <t>net_cash_from_operating_activities</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>6297553</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -662,7 +676,9 @@
           <t>capital_expenses</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>17662886</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -678,7 +694,9 @@
           <t>net_cash_from_investment_activities</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>-14596047</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -694,7 +712,9 @@
           <t>long_term_debt_principal_payments</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>1325000</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -718,7 +738,9 @@
           <t>net_cash_from_financing_activities</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>7533886</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -726,7 +748,9 @@
           <t>change_in_cash_and_equivalents</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>-764608</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -766,7 +790,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>76096</v>
+        <v>1608069</v>
       </c>
     </row>
     <row r="3">
@@ -776,7 +800,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45517</v>
+        <v>1128846</v>
       </c>
     </row>
     <row r="4">
@@ -802,7 +826,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-28308</v>
+        <v>1333220</v>
       </c>
     </row>
     <row r="7">
@@ -812,7 +836,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48839</v>
+        <v>1724357</v>
       </c>
     </row>
     <row r="8">
@@ -830,7 +854,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-18771</v>
+        <v>-202895</v>
       </c>
     </row>
     <row r="10">
@@ -848,7 +872,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>11431</v>
+        <v>225521</v>
       </c>
     </row>
     <row r="12">
@@ -874,7 +898,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>5335</v>
+        <v>196971</v>
       </c>
     </row>
     <row r="15">
@@ -884,7 +908,1271 @@
         </is>
       </c>
       <c r="B15" t="n">
+        <v>1327296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>873349</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>616748</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2811779</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>440257</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2151998</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>777016</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1152481</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2287902</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1295556.2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1371336</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>371819</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>440212</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8079347</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4220760</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>341011</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2761885</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10677588</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-8900915</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-11877590</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>10163015</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2161567</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1246407</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9147855</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>32150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>57046</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>30949</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>44103</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-54402</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>6065</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>6218</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-17235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>48539</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-11073</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-28308</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>48839</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-18771</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>11431</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5335</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>-41744</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1206282105.94</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>586407632.0700001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-3091426326.9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>920150736.05</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>277286556.04</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>956820491.0599999</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>613865951.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>157410000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3277592772.9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>463453002.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>2023-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>total_change_in_net_assets</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>215488</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>total_non_cash_exp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>258080</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>change_in_working_capital</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_operating_activities</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_operating_activities</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-1345762</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>capital_expenses</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>216236</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_investment_activities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_investment_activities</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>167725</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_net_proceeds</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>250552</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>long_term_debt_principal_payments</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>627260</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>change_in_long_term_debt</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-21785</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>other_changes_in_financing_activities</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>net_cash_from_financing_activities</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>change_in_cash_and_equivalents</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>-60232</v>
       </c>
     </row>
   </sheetData>
@@ -945,7 +2233,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-4315</v>
+        <v>-4826</v>
       </c>
     </row>
     <row r="5">
@@ -1021,7 +2309,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-345</v>
+        <v>-4345</v>
       </c>
     </row>
     <row r="13">
@@ -1090,7 +2378,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>323774</v>
+        <v>-502289</v>
       </c>
     </row>
     <row r="3">
@@ -1100,7 +2388,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>309720</v>
+        <v>748772</v>
       </c>
     </row>
     <row r="4">
@@ -1126,7 +2414,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18218</v>
+        <v>-7022740</v>
       </c>
     </row>
     <row r="7">
@@ -1136,7 +2424,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>358133</v>
+        <v>1113761</v>
       </c>
     </row>
     <row r="8">
@@ -1154,7 +2442,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-274848</v>
+        <v>1149921</v>
       </c>
     </row>
     <row r="10">
@@ -1164,7 +2452,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1269517</v>
+        <v>47245</v>
       </c>
     </row>
     <row r="11">
@@ -1174,7 +2462,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46070</v>
+        <v>365998</v>
       </c>
     </row>
     <row r="12">
@@ -1183,7 +2471,9 @@
           <t>change_in_long_term_debt</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>640013</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1200,7 +2490,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>205582</v>
+        <v>6764422</v>
       </c>
     </row>
     <row r="15">
@@ -1210,7 +2500,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-51048</v>
+        <v>38789</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +2541,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8395</v>
+        <v>488140</v>
       </c>
     </row>
     <row r="3">
@@ -1261,7 +2551,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7401</v>
+        <v>293011</v>
       </c>
     </row>
     <row r="4">
@@ -1286,7 +2576,9 @@
           <t>net_cash_from_operating_activities</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>-238803</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1294,7 +2586,9 @@
           <t>capital_expenses</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>504143</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1310,7 +2604,9 @@
           <t>net_cash_from_investment_activities</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>-464863</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1318,7 +2614,9 @@
           <t>long_term_debt_net_proceeds</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>1269517</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1326,7 +2624,9 @@
           <t>long_term_debt_principal_payments</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>738394</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1350,7 +2650,9 @@
           <t>net_cash_from_financing_activities</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>894914</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1358,7 +2660,9 @@
           <t>change_in_cash_and_equivalents</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>191248</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1398,7 +2702,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27296846</v>
+        <v>39322692</v>
       </c>
     </row>
     <row r="3">
@@ -1408,7 +2712,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12280.073</v>
+        <v>10112852</v>
       </c>
     </row>
     <row r="4">
@@ -1417,9 +2721,7 @@
           <t>change_in_working_capital</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>-4250119</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1436,7 +2738,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7320786</v>
+        <v>19904473</v>
       </c>
     </row>
     <row r="7">
@@ -1446,7 +2748,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18103845</v>
+        <v>11579120</v>
       </c>
     </row>
     <row r="8">
@@ -1455,9 +2757,7 @@
           <t>other_changes_in_investment_activities</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>-161868</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1466,7 +2766,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-13716182</v>
+        <v>-27266765</v>
       </c>
     </row>
     <row r="10">
@@ -1475,9 +2775,7 @@
           <t>long_term_debt_net_proceeds</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>550000</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1486,7 +2784,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2599642</v>
+        <v>5289884</v>
       </c>
     </row>
     <row r="12">
@@ -1503,9 +2801,7 @@
           <t>other_changes_in_financing_activities</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>246841</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1514,7 +2810,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-1475420</v>
+        <v>328207</v>
       </c>
     </row>
     <row r="15">
@@ -1524,7 +2820,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-7870816</v>
+        <v>-7034085</v>
       </c>
     </row>
   </sheetData>
@@ -1565,7 +2861,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6573828</v>
+        <v>8395</v>
       </c>
     </row>
     <row r="3">
@@ -1575,7 +2871,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8087552</v>
+        <v>7401</v>
       </c>
     </row>
     <row r="4">
@@ -1584,7 +2880,9 @@
           <t>change_in_working_capital</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>6555</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1601,7 +2899,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>14016100</v>
+        <v>12813</v>
       </c>
     </row>
     <row r="7">
@@ -1611,7 +2909,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2932101</v>
+        <v>10112</v>
       </c>
     </row>
     <row r="8">
@@ -1629,7 +2927,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>15262911</v>
+        <v>-9060</v>
       </c>
     </row>
     <row r="10">
@@ -1647,7 +2945,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2410000</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="12">
@@ -1656,7 +2954,9 @@
           <t>change_in_long_term_debt</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>-2402</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1664,7 +2964,9 @@
           <t>other_changes_in_financing_activities</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>1339</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1673,7 +2975,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-2120213</v>
+        <v>-792</v>
       </c>
     </row>
     <row r="15">
@@ -1683,7 +2985,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>27158798</v>
+        <v>2961</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +3026,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1608069000</v>
+        <v>23471502</v>
       </c>
     </row>
     <row r="3">
@@ -1734,7 +3036,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1128846000</v>
+        <v>12280.064</v>
       </c>
     </row>
     <row r="4">
@@ -1743,7 +3045,9 @@
           <t>change_in_working_capital</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>-4208019</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1760,7 +3064,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1333220000</v>
+        <v>7320786</v>
       </c>
     </row>
     <row r="7">
@@ -1770,7 +3074,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1724357000</v>
+        <v>18103845</v>
       </c>
     </row>
     <row r="8">
@@ -1788,7 +3092,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-202895000</v>
+        <v>-13716182</v>
       </c>
     </row>
     <row r="10">
@@ -1797,7 +3101,9 @@
           <t>long_term_debt_net_proceeds</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>550000</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1806,7 +3112,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>225521000</v>
+        <v>2599642</v>
       </c>
     </row>
     <row r="12">
@@ -1823,7 +3129,9 @@
           <t>other_changes_in_financing_activities</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>246841</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1832,7 +3140,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>196971000</v>
+        <v>-1475420</v>
       </c>
     </row>
     <row r="15">
@@ -1842,7 +3150,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1327296000</v>
+        <v>-7870816</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +3191,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2811779</v>
+        <v>342054</v>
       </c>
     </row>
     <row r="3">
@@ -1893,7 +3201,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>440257</v>
+        <v>238893</v>
       </c>
     </row>
     <row r="4">
@@ -1919,7 +3227,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-2151998</v>
+        <v>-537531</v>
       </c>
     </row>
     <row r="7">
@@ -1929,7 +3237,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>777016</v>
+        <v>328895</v>
       </c>
     </row>
     <row r="8">
@@ -1947,7 +3255,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1152481</v>
+        <v>207987</v>
       </c>
     </row>
     <row r="10">
@@ -1957,7 +3265,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2287902</v>
+        <v>466397</v>
       </c>
     </row>
     <row r="11">
@@ -1967,7 +3275,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1295464</v>
+        <v>190389</v>
       </c>
     </row>
     <row r="12">
@@ -1976,7 +3284,9 @@
           <t>change_in_long_term_debt</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>367558</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1993,7 +3303,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1371336</v>
+        <v>547395</v>
       </c>
     </row>
     <row r="15">
@@ -2003,7 +3313,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>371819</v>
+        <v>766454</v>
       </c>
     </row>
   </sheetData>
@@ -2044,7 +3354,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>440212</v>
+        <v>6573828</v>
       </c>
     </row>
     <row r="3">
@@ -2054,7 +3364,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8079347</v>
+        <v>8078552</v>
       </c>
     </row>
     <row r="4">
@@ -2063,9 +3373,7 @@
           <t>change_in_working_capital</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>3210760</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2073,9 +3381,7 @@
           <t>other_changes_in_operating_activities</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>341011</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2084,7 +3390,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2761885</v>
+        <v>14016100</v>
       </c>
     </row>
     <row r="7">
@@ -2094,7 +3400,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10677588</v>
+        <v>2932101</v>
       </c>
     </row>
     <row r="8">
@@ -2112,7 +3418,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-11877590</v>
+        <v>15262911</v>
       </c>
     </row>
     <row r="10">
@@ -2121,9 +3427,7 @@
           <t>long_term_debt_net_proceeds</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>10163015</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -2132,7 +3436,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2161567</v>
+        <v>2410000</v>
       </c>
     </row>
     <row r="12">
@@ -2149,9 +3453,7 @@
           <t>other_changes_in_financing_activities</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>1246407</v>
-      </c>
+      <c r="B13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -2160,7 +3462,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9147855</v>
+        <v>-2120213</v>
       </c>
     </row>
     <row r="15">
@@ -2170,7 +3472,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>32150</v>
+        <v>27158798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>